<commit_message>
added dependencies on russian gas
</commit_message>
<xml_diff>
--- a/Production&Demand.xlsx
+++ b/Production&Demand.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julik\PycharmProjects]\SERTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0416F43-4D5D-473E-9BF7-32540BE60CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B60DF0E7-E8A2-49A4-8F97-068D802D597F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="overview" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="57">
   <si>
     <t>Total 2021</t>
   </si>
@@ -201,13 +201,22 @@
   </si>
   <si>
     <t>unaccounted demand</t>
+  </si>
+  <si>
+    <t>Percentage Russian Gas</t>
+  </si>
+  <si>
+    <t>Moldavia</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,6 +229,17 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -239,15 +259,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Komma" xfId="1" builtinId="3"/>
+    <cellStyle name="Normal" xfId="2" xr:uid="{6D156F6E-D7F6-4053-9B71-504C2D2593A7}"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -475,8 +510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1809,18 +1844,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE7C4559-46EE-4210-9474-2BAE3F38DF6D}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.5546875" customWidth="1"/>
+    <col min="2" max="2" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>48</v>
       </c>
@@ -1834,610 +1874,747 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>17</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>96194000000</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="3">
         <v>30757000000</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="3">
         <v>64442000000</v>
       </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
+      <c r="E2" s="6">
+        <v>0.86</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3">
         <v>95547000000</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>18</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>186086000000</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>64994000000</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <v>110263000000</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="6">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F3" s="3">
         <v>3801000000</v>
       </c>
-      <c r="F3">
+      <c r="G3" s="3">
         <v>7610000000</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>19</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>2176000000</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>544000000</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <v>1733000000</v>
       </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E4" s="6">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>35325000000</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>14577000000</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <v>19708000000</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
+      <c r="E5" s="6">
+        <v>0.79</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
         <v>5803000000</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <v>29634000000</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <v>11315000000</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="3">
         <v>17888000000</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="6">
+        <v>0.16</v>
+      </c>
+      <c r="F6" s="3">
         <v>927000000</v>
       </c>
-      <c r="F6">
+      <c r="G6" s="3">
         <v>4773000000</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>100333000000</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <v>32361000000</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="3">
         <v>61838000000</v>
       </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
+      <c r="E7" s="6">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3">
         <v>43774000000</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>23</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <v>27688000000</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="3">
         <v>9323000000</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="3">
         <v>15528000000</v>
       </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
+      <c r="E8" s="7">
+        <f>0.66*E14</f>
+        <v>0.32340000000000002</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3">
         <v>9232000000</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>24</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>5123000000</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <v>1546000000</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="3">
         <v>3207000000</v>
       </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E9" s="6">
+        <v>0.12</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>25</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="3">
         <v>25088000000</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <v>8775000000</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="3">
         <v>10704000000</v>
       </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E10" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0</v>
+      </c>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>26</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="3">
         <v>474784000000</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="3">
         <v>135579000000</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="3">
         <v>318459000000</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="F11" s="3">
         <v>8871000000</v>
       </c>
-      <c r="F11">
+      <c r="G11" s="3">
         <v>132605000000</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>27</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="3">
         <v>4495000000</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="3">
         <v>1557000000</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="3">
         <v>2790000000</v>
       </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E12" s="6">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0</v>
+      </c>
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="6">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>28</v>
       </c>
-      <c r="B13">
+      <c r="B14" s="3">
         <v>1005600000000</v>
       </c>
-      <c r="C13">
+      <c r="C14" s="3">
         <v>331000000000</v>
       </c>
-      <c r="D13">
+      <c r="D14" s="3">
         <v>648500000000</v>
       </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
+      <c r="E14" s="6">
+        <v>0.49</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0</v>
+      </c>
+      <c r="G14" s="3">
         <v>245452000000</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>29</v>
       </c>
-      <c r="B14">
+      <c r="B15" s="3">
         <v>70150000000</v>
       </c>
-      <c r="C14">
+      <c r="C15" s="3">
         <v>35005000000</v>
       </c>
-      <c r="D14">
+      <c r="D15" s="3">
         <v>36240000000</v>
       </c>
-      <c r="E14">
+      <c r="E15" s="6">
+        <v>0.64</v>
+      </c>
+      <c r="F15" s="3">
         <v>1489000000</v>
       </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="G15" s="3">
+        <v>0</v>
+      </c>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>30</v>
       </c>
-      <c r="B15">
+      <c r="B16" s="3">
         <v>117477000000</v>
       </c>
-      <c r="C15">
+      <c r="C16" s="3">
         <v>35025000000</v>
       </c>
-      <c r="D15">
+      <c r="D16" s="3">
         <v>82033000000</v>
       </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
+      <c r="E16" s="6">
+        <v>0.61</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3">
         <v>67703000000</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>31</v>
       </c>
-      <c r="B16">
+      <c r="B17" s="3">
         <v>55073000000</v>
       </c>
-      <c r="C16">
+      <c r="C17" s="3">
         <v>25352000000</v>
       </c>
-      <c r="D16">
+      <c r="D17" s="3">
         <v>28719000000</v>
       </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="E17" s="7">
+        <f>0.7*E32</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0</v>
+      </c>
+      <c r="I17" s="4"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>32</v>
       </c>
-      <c r="B17">
+      <c r="B18" s="3">
         <v>799401000000</v>
       </c>
-      <c r="C17">
+      <c r="C18" s="3">
         <v>294365000000</v>
       </c>
-      <c r="D17">
+      <c r="D18" s="3">
         <v>507127000000</v>
       </c>
-      <c r="E17">
+      <c r="E18" s="6">
+        <v>0.38</v>
+      </c>
+      <c r="F18" s="3">
         <v>3059000000</v>
       </c>
-      <c r="F17">
+      <c r="G18" s="3">
         <v>193443000000</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="I18" s="4"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>33</v>
       </c>
-      <c r="B18">
+      <c r="B19" s="3">
         <v>12526000000</v>
       </c>
-      <c r="C18">
+      <c r="C19" s="3">
         <v>3371000000</v>
       </c>
-      <c r="D18">
+      <c r="D19" s="3">
         <v>7495000000</v>
       </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
+      <c r="E19" s="6">
+        <v>0.92</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0</v>
+      </c>
+      <c r="G19" s="3">
         <v>24074000000</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="I19" s="4"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>34</v>
       </c>
-      <c r="B19">
+      <c r="B20" s="3">
         <v>24186000000</v>
       </c>
-      <c r="C19">
+      <c r="C20" s="3">
         <v>9846000000</v>
       </c>
-      <c r="D19">
+      <c r="D20" s="3">
         <v>11345000000</v>
       </c>
-      <c r="E19">
+      <c r="E20" s="6">
+        <v>0.27</v>
+      </c>
+      <c r="F20" s="3">
         <v>1094000000</v>
       </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="G20" s="3">
+        <v>0</v>
+      </c>
+      <c r="I20" s="4"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>35</v>
       </c>
-      <c r="B20">
+      <c r="B21" s="3">
         <v>8655000000</v>
       </c>
-      <c r="C20">
+      <c r="C21" s="3">
         <v>3079000000</v>
       </c>
-      <c r="D20">
+      <c r="D21" s="3">
         <v>5311000000</v>
       </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="E21" s="7"/>
+      <c r="F21" s="3">
+        <v>0</v>
+      </c>
+      <c r="G21" s="3">
+        <v>0</v>
+      </c>
+      <c r="I21" s="4"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>36</v>
       </c>
-      <c r="B21">
+      <c r="B22" s="3">
         <v>382742000000</v>
       </c>
-      <c r="C21">
+      <c r="C22" s="3">
         <v>145003000000</v>
       </c>
-      <c r="D21">
+      <c r="D22" s="3">
         <v>205786000000</v>
       </c>
-      <c r="E21">
+      <c r="E22" s="7">
+        <f>0.18*E14</f>
+        <v>8.8200000000000001E-2</v>
+      </c>
+      <c r="F22" s="3">
         <v>4602000000</v>
       </c>
-      <c r="F21">
+      <c r="G22" s="3">
         <v>138991000000</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="I22" s="4"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>37</v>
       </c>
-      <c r="B22">
+      <c r="B23" s="3">
         <v>207616000000</v>
       </c>
-      <c r="C22">
+      <c r="C23" s="3">
         <v>79297000000</v>
       </c>
-      <c r="D22">
+      <c r="D23" s="3">
         <v>119400000000</v>
       </c>
-      <c r="E22">
+      <c r="E23" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F23" s="3">
         <v>2118000000</v>
       </c>
-      <c r="F22">
+      <c r="G23" s="3">
         <v>36410000000</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="I23" s="4"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>38</v>
       </c>
-      <c r="B23">
+      <c r="B24" s="3">
         <v>61683000000</v>
       </c>
-      <c r="C23">
+      <c r="C24" s="3">
         <v>31793000000</v>
       </c>
-      <c r="D23">
+      <c r="D24" s="3">
         <v>30831000000</v>
       </c>
-      <c r="E23">
+      <c r="E24" s="7">
+        <v>0</v>
+      </c>
+      <c r="F24" s="3">
         <v>2582000000</v>
       </c>
-      <c r="F23">
+      <c r="G24" s="3">
         <v>3670000000</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="I24" s="4"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>39</v>
       </c>
-      <c r="B24">
+      <c r="B25" s="3">
         <v>119742000000</v>
       </c>
-      <c r="C24">
+      <c r="C25" s="3">
         <v>36546000000</v>
       </c>
-      <c r="D24">
+      <c r="D25" s="3">
         <v>78334000000</v>
       </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
+      <c r="E25" s="6">
+        <v>0.24</v>
+      </c>
+      <c r="F25" s="3">
+        <v>0</v>
+      </c>
+      <c r="G25" s="3">
         <v>32794000000</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="I25" s="4"/>
+      <c r="J25" s="5"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>40</v>
       </c>
-      <c r="B25">
-        <v>0</v>
-      </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="B26" s="3">
+        <v>0</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0</v>
+      </c>
+      <c r="D26" s="3">
+        <v>0</v>
+      </c>
+      <c r="E26" s="6">
+        <v>0.89</v>
+      </c>
+      <c r="F26" s="3">
+        <v>0</v>
+      </c>
+      <c r="G26" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>41</v>
       </c>
-      <c r="B26">
+      <c r="B27" s="3">
         <v>59227000000</v>
       </c>
-      <c r="C26">
+      <c r="C27" s="3">
         <v>19446000000</v>
       </c>
-      <c r="D26">
+      <c r="D27" s="3">
         <v>37406000000</v>
       </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="F26">
+      <c r="E27" s="6">
+        <v>0.68</v>
+      </c>
+      <c r="F27" s="3">
+        <v>0</v>
+      </c>
+      <c r="G27" s="3">
         <v>35048000000</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>42</v>
       </c>
-      <c r="B27">
+      <c r="B28" s="3">
         <v>10186000000</v>
       </c>
-      <c r="C27">
+      <c r="C28" s="3">
         <v>3808000000</v>
       </c>
-      <c r="D27">
+      <c r="D28" s="3">
         <v>6307000000</v>
       </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="E28" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="F28" s="3">
+        <v>0</v>
+      </c>
+      <c r="G28" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>43</v>
       </c>
-      <c r="B28">
+      <c r="B29" s="3">
         <v>378297000000</v>
       </c>
-      <c r="C28">
+      <c r="C29" s="3">
         <v>170578000000</v>
       </c>
-      <c r="D28">
+      <c r="D29" s="3">
         <v>219170000000</v>
       </c>
-      <c r="E28">
+      <c r="E29" s="7">
+        <v>0</v>
+      </c>
+      <c r="F29" s="3">
         <v>21955000000</v>
       </c>
-      <c r="F28">
+      <c r="G29" s="3">
         <v>3500000000</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>44</v>
       </c>
-      <c r="B29">
+      <c r="B30" s="3">
         <v>8916000000</v>
       </c>
-      <c r="C29">
+      <c r="C30" s="3">
         <v>3205000000</v>
       </c>
-      <c r="D29">
+      <c r="D30" s="3">
         <v>4596000000</v>
       </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29">
+      <c r="E30" s="7">
+        <f>E8</f>
+        <v>0.32340000000000002</v>
+      </c>
+      <c r="F30" s="3">
+        <v>0</v>
+      </c>
+      <c r="G30" s="3">
         <v>101000000</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>46</v>
       </c>
-      <c r="B30">
+      <c r="B31" s="3">
         <v>35404000000</v>
       </c>
-      <c r="C30">
+      <c r="C31" s="3">
         <v>8975000000</v>
       </c>
-      <c r="D30">
+      <c r="D31" s="3">
         <v>26084000000</v>
       </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="E31" s="7"/>
+      <c r="F31" s="3">
+        <v>0</v>
+      </c>
+      <c r="G31" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>47</v>
       </c>
-      <c r="B31">
+      <c r="B32" s="3">
         <v>855671000000</v>
       </c>
-      <c r="C31">
+      <c r="C32" s="3">
         <v>346509000000</v>
       </c>
-      <c r="D31">
+      <c r="D32" s="3">
         <v>446604000000</v>
       </c>
-      <c r="E31">
-        <v>0</v>
-      </c>
-      <c r="F31">
+      <c r="E32" s="7">
+        <v>0</v>
+      </c>
+      <c r="F32" s="3">
+        <v>0</v>
+      </c>
+      <c r="G32" s="3">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
minor fixes and corrections in the db
</commit_message>
<xml_diff>
--- a/Production&Demand.xlsx
+++ b/Production&Demand.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julik\PycharmProjects]\SERTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B60DF0E7-E8A2-49A4-8F97-068D802D597F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D8C4F5-E6A4-4547-A924-F6266344AF69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="58">
   <si>
     <t>Total 2021</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>Moldavia</t>
+  </si>
+  <si>
+    <t>*</t>
   </si>
 </sst>
 </file>
@@ -275,7 +278,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -1844,10 +1847,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE7C4559-46EE-4210-9474-2BAE3F38DF6D}">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2255,7 +2258,7 @@
         <v>28719000000</v>
       </c>
       <c r="E17" s="7">
-        <f>0.7*E32</f>
+        <f>0.7*E33</f>
         <v>0</v>
       </c>
       <c r="F17" s="3">
@@ -2463,7 +2466,7 @@
         <v>40</v>
       </c>
       <c r="B26" s="3">
-        <v>0</v>
+        <v>12867000000</v>
       </c>
       <c r="C26" s="3">
         <v>0</v>
@@ -2479,6 +2482,9 @@
       </c>
       <c r="G26" s="3">
         <v>0</v>
+      </c>
+      <c r="H26" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -2597,24 +2603,42 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" s="3">
+        <v>344541000000</v>
+      </c>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="7">
+        <v>0.45</v>
+      </c>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>47</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B33" s="3">
         <v>855671000000</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C33" s="3">
         <v>346509000000</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D33" s="3">
         <v>446604000000</v>
       </c>
-      <c r="E32" s="7">
-        <v>0</v>
-      </c>
-      <c r="F32" s="3">
-        <v>0</v>
-      </c>
-      <c r="G32" s="3">
+      <c r="E33" s="7">
+        <v>0</v>
+      </c>
+      <c r="F33" s="3">
+        <v>0</v>
+      </c>
+      <c r="G33" s="3">
         <v>0</v>
       </c>
     </row>

</xml_diff>